<commit_message>
Updated all output figures to latest code
</commit_message>
<xml_diff>
--- a/results/tables/sctype_scores.xlsx
+++ b/results/tables/sctype_scores.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">cluster</t>
   </si>
@@ -26,118 +26,145 @@
     <t xml:space="preserve">ncells</t>
   </si>
   <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erythroid-like and erythroid precursor cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-classical monocytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memory CD4+ T cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classical Monocytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progenitor cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD8+ NKT-like cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naive CD4+ T cells</t>
+  </si>
+  <si>
     <t xml:space="preserve">8</t>
   </si>
   <si>
-    <t xml:space="preserve">Erythroid-like and erythroid precursor cells</t>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro-B cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plasmacytoid Dendritic cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naive B cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutrophils</t>
   </si>
   <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-classical monocytes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naive CD8+ T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classical Monocytes</t>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myeloid Dendritic cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plasma B cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basophils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platelets</t>
   </si>
   <si>
     <t xml:space="preserve">7</t>
   </si>
   <si>
-    <t xml:space="preserve">Progenitor cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ NKT-like cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural killer  cells</t>
+    <t xml:space="preserve">25</t>
   </si>
   <si>
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pro-B cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plasmacytoid Dendritic cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Immature B cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neutrophils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myeloid Dendritic cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plasma B cells</t>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-B cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
   </si>
   <si>
     <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naive CD4+ T cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endothelial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-B cells</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
   </si>
 </sst>
 </file>
@@ -491,10 +518,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>4516.16898071339</v>
+        <v>2885.69050364</v>
       </c>
       <c r="D2" t="n">
-        <v>2455</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="3">
@@ -505,10 +532,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>10358.0164008351</v>
+        <v>8769.14800576094</v>
       </c>
       <c r="D3" t="n">
-        <v>1530</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="4">
@@ -519,10 +546,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>7872.68054573931</v>
+        <v>5842.30365969639</v>
       </c>
       <c r="D4" t="n">
-        <v>21845</v>
+        <v>7171</v>
       </c>
     </row>
     <row r="5">
@@ -533,10 +560,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>43177.6497699998</v>
+        <v>29659.4117541113</v>
       </c>
       <c r="D5" t="n">
-        <v>7051</v>
+        <v>6454</v>
       </c>
     </row>
     <row r="6">
@@ -547,10 +574,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>11307.5278831742</v>
+        <v>6787.16150937724</v>
       </c>
       <c r="D6" t="n">
-        <v>2485</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="7">
@@ -561,63 +588,63 @@
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>35708.2770378851</v>
+        <v>14781.6568718554</v>
       </c>
       <c r="D7" t="n">
-        <v>11557</v>
+        <v>7170</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="n">
-        <v>35708.2770378851</v>
+        <v>7842.64865883329</v>
       </c>
       <c r="D8" t="n">
-        <v>11557</v>
+        <v>13649</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>18924.6495659206</v>
+        <v>12441.3066716757</v>
       </c>
       <c r="D9" t="n">
-        <v>3773</v>
+        <v>3006</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>14431.5855097465</v>
+        <v>10098.2594569949</v>
       </c>
       <c r="D10" t="n">
-        <v>1434</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>6429.31374552643</v>
+        <v>5588.86517671047</v>
       </c>
       <c r="D11" t="n">
         <v>704</v>
@@ -625,16 +652,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>18612.8385394539</v>
+        <v>4752.28370843202</v>
       </c>
       <c r="D12" t="n">
-        <v>4829</v>
+        <v>598</v>
       </c>
     </row>
     <row r="13">
@@ -642,55 +669,55 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C13" t="n">
-        <v>7122.07890924765</v>
+        <v>16008.056248344</v>
       </c>
       <c r="D13" t="n">
-        <v>2114</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C14" t="n">
-        <v>11323.0467983177</v>
+        <v>6372.67385789029</v>
       </c>
       <c r="D14" t="n">
-        <v>2860</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>7581.4042857172</v>
+        <v>5849.20801437865</v>
       </c>
       <c r="D15" t="n">
-        <v>1114</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>6952.33426434563</v>
+        <v>8911.97250239573</v>
       </c>
       <c r="D16" t="n">
-        <v>1323</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="17">
@@ -701,10 +728,10 @@
         <v>31</v>
       </c>
       <c r="C17" t="n">
-        <v>5322.28716251285</v>
+        <v>5418.40023556216</v>
       </c>
       <c r="D17" t="n">
-        <v>774</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="18">
@@ -712,83 +739,83 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C18" t="n">
-        <v>836.079925624319</v>
+        <v>5114.55932054654</v>
       </c>
       <c r="D18" t="n">
-        <v>263</v>
+        <v>774</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C19" t="n">
-        <v>836.079925624319</v>
+        <v>2168.05087507139</v>
       </c>
       <c r="D19" t="n">
-        <v>263</v>
+        <v>641</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C20" t="n">
-        <v>382.94498277719</v>
+        <v>820.165921918189</v>
       </c>
       <c r="D20" t="n">
-        <v>987</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C21" t="n">
-        <v>3291.50807559994</v>
+        <v>17992.6925214684</v>
       </c>
       <c r="D21" t="n">
-        <v>8315</v>
+        <v>4892</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>135.763900068149</v>
+        <v>3259.6751951709</v>
       </c>
       <c r="D22" t="n">
-        <v>27</v>
+        <v>763</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="C23" t="n">
-        <v>313.688252020679</v>
+        <v>833.358392979185</v>
       </c>
       <c r="D23" t="n">
-        <v>148</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="24">
@@ -796,27 +823,125 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C24" t="n">
-        <v>477.024858046482</v>
+        <v>940.514407716718</v>
       </c>
       <c r="D24" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="n">
+        <v>3191.83225863921</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3883</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="n">
-        <v>2138.88600904855</v>
-      </c>
-      <c r="D25" t="n">
-        <v>925</v>
+      <c r="C26" t="n">
+        <v>353.934289117898</v>
+      </c>
+      <c r="D26" t="n">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="n">
+        <v>5166.73686458309</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="n">
+        <v>357.311828286381</v>
+      </c>
+      <c r="D28" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="n">
+        <v>264.309117078594</v>
+      </c>
+      <c r="D29" t="n">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="n">
+        <v>331.543501376462</v>
+      </c>
+      <c r="D30" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="n">
+        <v>3033.43229932265</v>
+      </c>
+      <c r="D31" t="n">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1605.86502126487</v>
+      </c>
+      <c r="D32" t="n">
+        <v>930</v>
       </c>
     </row>
   </sheetData>

</xml_diff>